<commit_message>
Update with GW10 data
</commit_message>
<xml_diff>
--- a/results/Player_Analysis_Dashboard_2023_24.xlsx
+++ b/results/Player_Analysis_Dashboard_2023_24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Development\Desktop\Fantasy Football\PL-Analysis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76527F7E-C848-42D4-A365-48F05207F5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB4EFA3-97F6-42A4-94CD-FCCD481DD768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GK" sheetId="1" r:id="rId1"/>
@@ -76,22 +76,22 @@
     <t>Alisson Ramses Becker</t>
   </si>
   <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>David Raya Martin</t>
+  </si>
+  <si>
+    <t>Jason Steele</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Ederson Santana de Moraes</t>
+  </si>
+  <si>
     <t>Very small</t>
-  </si>
-  <si>
-    <t>David Raya Martin</t>
-  </si>
-  <si>
-    <t>Small</t>
-  </si>
-  <si>
-    <t>Jason Steele</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Ederson Santana de Moraes</t>
   </si>
   <si>
     <t>José Malheiro de Sá</t>
@@ -433,7 +433,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="52">
+  <fills count="59">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,11 +462,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCECE6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF98D8C9"/>
       </patternFill>
     </fill>
@@ -477,32 +472,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCCECE6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE5F5F9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8A4A9"/>
+        <fgColor rgb="FFE6959B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE4888F"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2777F"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDC4C56"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE4868D"/>
+        <fgColor rgb="FFDB4550"/>
       </patternFill>
     </fill>
     <fill>
@@ -512,17 +497,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDF616B"/>
+        <fgColor rgb="FFE27981"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE16E77"/>
+        <fgColor rgb="FFDC4A55"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE06871"/>
+        <fgColor rgb="FFDF636C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD505A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE37C84"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDE5963"/>
       </patternFill>
     </fill>
     <fill>
@@ -537,12 +537,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F1F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFEFDBDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0E0E1"/>
+        <fgColor rgb="FFEED0D2"/>
       </patternFill>
     </fill>
     <fill>
@@ -552,7 +557,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEECDCF"/>
+        <fgColor rgb="FFECC0C3"/>
       </patternFill>
     </fill>
     <fill>
@@ -562,12 +567,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F1F1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE9ACB1"/>
+        <fgColor rgb="FFE8A1A6"/>
       </patternFill>
     </fill>
     <fill>
@@ -577,7 +577,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6959B"/>
+        <fgColor rgb="FFEBBBBE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E7DF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9A8AD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEECDCF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0E1E2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB9D3C5"/>
       </patternFill>
     </fill>
     <fill>
@@ -587,42 +612,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD7E6DE"/>
+        <fgColor rgb="FFE9ABAF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE9A8AD"/>
+        <fgColor rgb="FFE59097"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE79CA2"/>
+        <fgColor rgb="FFDE5660"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE4838B"/>
+        <fgColor rgb="FFE69399"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDF646D"/>
+        <fgColor rgb="FFE4868D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE58B91"/>
+        <fgColor rgb="FFDF6069"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDD535D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE79A9F"/>
+        <fgColor rgb="FFDD4F59"/>
       </patternFill>
     </fill>
     <fill>
@@ -632,32 +652,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6979D"/>
+        <fgColor rgb="FFE06A73"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEDCCCE"/>
+        <fgColor rgb="FFE2777F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7EFEA"/>
+        <fgColor rgb="FFE58D94"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFECC3C6"/>
+        <fgColor rgb="FFE0656F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEDC7CA"/>
+        <fgColor rgb="FFF0DEDF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDD505A"/>
+        <fgColor rgb="FFE27880"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6E5DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAB3B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDE5B65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD515C"/>
       </patternFill>
     </fill>
     <fill>
@@ -667,27 +707,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDC4752"/>
+        <fgColor rgb="FF84B29A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE27880"/>
+        <fgColor rgb="FFEFD4D6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE48990"/>
+        <fgColor rgb="FFE9A9AE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEBBBBE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF589776"/>
+        <fgColor rgb="FFEBB8BB"/>
       </patternFill>
     </fill>
   </fills>
@@ -718,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -726,10 +761,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -742,37 +777,44 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1083,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1092,47 +1134,47 @@
     <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="53" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52" t="s">
+    <row r="1" spans="1:14" s="60" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="59" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1191,22 +1233,22 @@
         <v>2.6</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3">
-        <v>3.7</v>
+        <v>3.64</v>
       </c>
       <c r="G3">
-        <v>-0.2</v>
+        <v>-0.22</v>
       </c>
       <c r="H3">
-        <v>0.82</v>
+        <v>0.78</v>
       </c>
       <c r="I3">
-        <v>-0.63</v>
+        <v>-0.74</v>
       </c>
       <c r="J3">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="K3" s="3" t="b">
         <v>0</v>
@@ -1215,10 +1257,10 @@
         <v>17</v>
       </c>
       <c r="M3" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="N3" s="7">
-        <v>3.1</v>
+        <v>5.6</v>
+      </c>
+      <c r="N3" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1235,39 +1277,39 @@
         <v>2.11</v>
       </c>
       <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8">
-        <v>4.67</v>
+        <v>7</v>
+      </c>
+      <c r="F4" s="7">
+        <v>4.29</v>
       </c>
       <c r="G4">
-        <v>0.41</v>
+        <v>0.23</v>
       </c>
       <c r="H4">
-        <v>0.86</v>
+        <v>0.8</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="J4">
-        <v>0.18</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>19</v>
+      <c r="L4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M4" s="2">
         <v>4.8</v>
       </c>
-      <c r="N4" s="10">
-        <v>3.17</v>
+      <c r="N4" s="8">
+        <v>3.29</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>16</v>
@@ -1299,19 +1341,19 @@
       <c r="K5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>21</v>
+      <c r="L5" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M5" s="2">
         <v>4.3</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="10">
         <v>3.33</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>72</v>
@@ -1323,34 +1365,34 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="E6">
-        <v>9</v>
-      </c>
-      <c r="F6" s="8">
-        <v>3.78</v>
+        <v>10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.6</v>
       </c>
       <c r="G6">
-        <v>0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="H6">
-        <v>0.75</v>
+        <v>0.71</v>
       </c>
       <c r="I6">
-        <v>0.15</v>
+        <v>-0.09</v>
       </c>
       <c r="J6">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="K6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>17</v>
+      <c r="L6" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M6" s="2">
         <v>5.5</v>
       </c>
-      <c r="N6" s="13">
-        <v>3.11</v>
+      <c r="N6" s="12">
+        <v>3.1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1367,34 +1409,34 @@
         <v>2.71</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="3">
-        <v>2.9</v>
+        <v>2.73</v>
       </c>
       <c r="G7">
-        <v>-0.27</v>
+        <v>-0.33</v>
       </c>
       <c r="H7">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="I7">
-        <v>-0.85</v>
+        <v>-1.1100000000000001</v>
       </c>
       <c r="J7">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="K7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>19</v>
+      <c r="L7" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
-      <c r="N7" s="14">
-        <v>3.4</v>
+      <c r="N7" s="13">
+        <v>3.27</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1411,34 +1453,34 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8" s="8">
-        <v>3.7</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="7">
+        <v>3.91</v>
       </c>
       <c r="G8">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="H8">
-        <v>0.72</v>
+        <v>0.69</v>
       </c>
       <c r="I8">
-        <v>0.17</v>
+        <v>0.49</v>
       </c>
       <c r="J8">
-        <v>0.43</v>
+        <v>0.32</v>
       </c>
       <c r="K8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>17</v>
+      <c r="L8" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M8" s="2">
         <v>5.5</v>
       </c>
-      <c r="N8" s="7">
-        <v>3.1</v>
+      <c r="N8" s="14">
+        <v>3.18</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1475,11 +1517,11 @@
       <c r="K9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>19</v>
+      <c r="L9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M9" s="2">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="N9" s="15">
         <v>3.25</v>
@@ -1499,34 +1541,34 @@
         <v>2.7</v>
       </c>
       <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10" s="8">
-        <v>3.5</v>
+        <v>11</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3.82</v>
       </c>
       <c r="G10">
-        <v>0.02</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H10">
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="I10">
-        <v>7.0000000000000007E-2</v>
+        <v>0.46</v>
       </c>
       <c r="J10">
-        <v>0.47</v>
+        <v>0.33</v>
       </c>
       <c r="K10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>17</v>
+      <c r="L10" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M10" s="2">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N10" s="16">
-        <v>3.2</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1543,34 +1585,34 @@
         <v>2.13</v>
       </c>
       <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" s="8">
-        <v>3.5</v>
+        <v>11</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3.45</v>
       </c>
       <c r="G11">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="H11">
-        <v>0.67</v>
+        <v>0.64</v>
       </c>
       <c r="I11">
-        <v>0.19</v>
+        <v>0.12</v>
       </c>
       <c r="J11">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="K11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>17</v>
+      <c r="L11" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M11" s="2">
         <v>4.7</v>
       </c>
-      <c r="N11" s="7">
-        <v>3.1</v>
+      <c r="N11" s="14">
+        <v>3.18</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1587,34 +1629,34 @@
         <v>2.56</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3">
-        <v>2.56</v>
+        <v>2.4</v>
       </c>
       <c r="G12">
-        <v>-0.3</v>
+        <v>-0.36</v>
       </c>
       <c r="H12">
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="I12">
-        <v>-0.91</v>
+        <v>-1.1499999999999999</v>
       </c>
       <c r="J12">
-        <v>0.19</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="9" t="s">
-        <v>19</v>
+      <c r="L12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M12" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N12" s="13">
-        <v>3.11</v>
+      <c r="N12" s="12">
+        <v>3.1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1631,28 +1673,28 @@
         <v>2.21</v>
       </c>
       <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13" s="8">
-        <v>3.4</v>
+        <v>11</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3.36</v>
       </c>
       <c r="G13">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="H13">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="I13">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="J13">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="K13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>17</v>
+      <c r="L13" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M13" s="2">
         <v>4.5999999999999996</v>
@@ -1695,8 +1737,8 @@
       <c r="K14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>17</v>
+      <c r="L14" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M14" s="2">
         <v>4.5</v>
@@ -1719,28 +1761,28 @@
         <v>2.04</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" s="3">
-        <v>2.5</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="G15">
-        <v>-0.26</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="H15">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="I15">
-        <v>-0.82</v>
+        <v>-0.93</v>
       </c>
       <c r="J15">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="K15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="9" t="s">
-        <v>19</v>
+      <c r="L15" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M15" s="2">
         <v>4.4000000000000004</v>
@@ -1800,7 +1842,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1808,47 +1850,47 @@
     <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="53" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52" t="s">
+    <row r="1" spans="1:14" s="60" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="59" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1866,34 +1908,34 @@
         <v>3.33</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>3.25</v>
+        <v>3.11</v>
       </c>
       <c r="G2">
-        <v>-0.38</v>
+        <v>-0.42</v>
       </c>
       <c r="H2">
-        <v>1.18</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="I2">
-        <v>-1.07</v>
+        <v>-1.26</v>
       </c>
       <c r="J2">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="K2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>19</v>
+      <c r="L2" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M2" s="2">
         <v>7.9</v>
       </c>
       <c r="N2" s="20">
-        <v>3.12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -1930,13 +1972,13 @@
       <c r="K3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>19</v>
+      <c r="L3" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M3" s="2">
         <v>6.5</v>
       </c>
-      <c r="N3" s="20">
+      <c r="N3" s="21">
         <v>3.12</v>
       </c>
     </row>
@@ -1954,34 +1996,34 @@
         <v>3.23</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>2.88</v>
+        <v>2.78</v>
       </c>
       <c r="G4">
-        <v>-0.44</v>
+        <v>-0.47</v>
       </c>
       <c r="H4">
-        <v>1.1399999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="I4">
-        <v>-1.25</v>
+        <v>-1.41</v>
       </c>
       <c r="J4">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="K4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>19</v>
+      <c r="L4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M4" s="2">
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="N4" s="20">
-        <v>3.12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -2015,7 +2057,7 @@
       <c r="K5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="2">
@@ -2039,22 +2081,22 @@
         <v>2.77</v>
       </c>
       <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" s="8">
-        <v>4.7</v>
+        <v>11</v>
+      </c>
+      <c r="F6" s="7">
+        <v>4.82</v>
       </c>
       <c r="G6">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
       <c r="H6">
-        <v>0.88</v>
+        <v>0.84</v>
       </c>
       <c r="I6">
-        <v>0.59</v>
+        <v>0.76</v>
       </c>
       <c r="J6">
-        <v>0.28000000000000003</v>
+        <v>0.23</v>
       </c>
       <c r="K6" s="3" t="b">
         <v>0</v>
@@ -2065,8 +2107,8 @@
       <c r="M6" s="2">
         <v>7</v>
       </c>
-      <c r="N6" s="22">
-        <v>3.1</v>
+      <c r="N6" s="23">
+        <v>3.18</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -2103,13 +2145,13 @@
       <c r="K7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="11" t="s">
-        <v>21</v>
+      <c r="L7" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M7" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="24">
         <v>3.14</v>
       </c>
     </row>
@@ -2127,34 +2169,34 @@
         <v>2.93</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="3">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="G8">
-        <v>-0.32</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="H8">
-        <v>1.69</v>
+        <v>1.47</v>
       </c>
       <c r="I8">
-        <v>-0.56000000000000005</v>
+        <v>-0.13</v>
       </c>
       <c r="J8">
-        <v>0.32</v>
+        <v>0.45</v>
       </c>
       <c r="K8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>19</v>
+      <c r="L8" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M8" s="2">
         <v>5.3</v>
       </c>
-      <c r="N8" s="10">
-        <v>3.67</v>
+      <c r="N8" s="5">
+        <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -2171,34 +2213,34 @@
         <v>3.36</v>
       </c>
       <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="8">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>3.82</v>
       </c>
       <c r="G9">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1.06</v>
+        <v>1.01</v>
       </c>
       <c r="I9">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
       <c r="K9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>17</v>
+      <c r="L9" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="M9" s="2">
         <v>5.2</v>
       </c>
-      <c r="N9" s="24">
-        <v>3.2</v>
+      <c r="N9" s="25">
+        <v>3.27</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -2235,13 +2277,13 @@
       <c r="K10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="11" t="s">
-        <v>21</v>
+      <c r="L10" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M10" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="26">
         <v>3.33</v>
       </c>
     </row>
@@ -2259,34 +2301,34 @@
         <v>4.4400000000000004</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="3">
-        <v>1.33</v>
+        <v>1.5</v>
       </c>
       <c r="G11">
-        <v>-0.53</v>
+        <v>-0.49</v>
       </c>
       <c r="H11">
-        <v>2.57</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="I11">
-        <v>-0.91</v>
+        <v>-0.98</v>
       </c>
       <c r="J11">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="K11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="11" t="s">
-        <v>21</v>
+      <c r="L11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M11" s="2">
         <v>5.3</v>
       </c>
-      <c r="N11" s="10">
-        <v>3.67</v>
+      <c r="N11" s="5">
+        <v>3.5</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -2303,33 +2345,33 @@
         <v>3.6</v>
       </c>
       <c r="E12">
-        <v>9</v>
-      </c>
-      <c r="F12" s="8">
-        <v>4.1100000000000003</v>
+        <v>10</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3.7</v>
       </c>
       <c r="G12">
-        <v>0.14000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="H12">
-        <v>1.2</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I12">
-        <v>0.43</v>
+        <v>0.09</v>
       </c>
       <c r="J12">
-        <v>0.34</v>
+        <v>0.47</v>
       </c>
       <c r="K12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="6" t="s">
-        <v>17</v>
+      <c r="L12" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M12" s="2">
         <v>5.2</v>
       </c>
-      <c r="N12" s="26">
+      <c r="N12" s="20">
         <v>3</v>
       </c>
     </row>
@@ -2347,34 +2389,34 @@
         <v>3.28</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F13" s="3">
-        <v>2.88</v>
+        <v>2.78</v>
       </c>
       <c r="G13">
-        <v>-0.21</v>
+        <v>-0.24</v>
       </c>
       <c r="H13">
-        <v>1.1599999999999999</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I13">
-        <v>-0.6</v>
+        <v>-0.73</v>
       </c>
       <c r="J13">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="K13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="9" t="s">
-        <v>19</v>
+      <c r="L13" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M13" s="2">
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
       <c r="N13" s="27">
-        <v>3.38</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2411,8 +2453,8 @@
       <c r="K14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L14" s="9" t="s">
-        <v>19</v>
+      <c r="L14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M14" s="2">
         <v>4.3</v>
@@ -2435,34 +2477,34 @@
         <v>3.12</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="3">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
       <c r="G15">
-        <v>-0.64</v>
+        <v>-0.69</v>
       </c>
       <c r="H15">
-        <v>2.21</v>
+        <v>1.8</v>
       </c>
       <c r="I15">
-        <v>-0.91</v>
+        <v>-1.2</v>
       </c>
       <c r="J15">
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
       <c r="K15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="11" t="s">
-        <v>21</v>
+      <c r="L15" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M15" s="2">
         <v>4.8</v>
       </c>
-      <c r="N15" s="29">
-        <v>3.5</v>
+      <c r="N15" s="26">
+        <v>3.33</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -2479,34 +2521,34 @@
         <v>2.86</v>
       </c>
       <c r="E16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>3.22</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>-0.09</v>
+        <v>-0.17</v>
       </c>
       <c r="H16">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="I16">
-        <v>-0.27</v>
+        <v>-0.53</v>
       </c>
       <c r="J16">
-        <v>0.4</v>
+        <v>0.31</v>
       </c>
       <c r="K16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>17</v>
+      <c r="L16" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M16" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N16" s="30">
-        <v>3.22</v>
+      <c r="N16" s="29">
+        <v>3.3</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -2523,34 +2565,34 @@
         <v>2.82</v>
       </c>
       <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="F17" s="3">
-        <v>3.4</v>
+        <v>11</v>
+      </c>
+      <c r="F17" s="7">
+        <v>3.55</v>
       </c>
       <c r="G17">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="H17">
-        <v>0.89</v>
+        <v>0.85</v>
       </c>
       <c r="I17">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J17">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="K17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L17" s="6" t="s">
-        <v>17</v>
+      <c r="L17" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M17" s="2">
         <v>5.2</v>
       </c>
-      <c r="N17" s="22">
-        <v>3.1</v>
+      <c r="N17" s="23">
+        <v>3.18</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -2567,34 +2609,34 @@
         <v>2.48</v>
       </c>
       <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18" s="8">
-        <v>4.4000000000000004</v>
+        <v>11</v>
+      </c>
+      <c r="F18" s="7">
+        <v>4.18</v>
       </c>
       <c r="G18">
-        <v>0.38</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H18">
-        <v>0.79</v>
+        <v>0.75</v>
       </c>
       <c r="I18">
-        <v>1.2</v>
+        <v>0.97</v>
       </c>
       <c r="J18">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="K18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="9" t="s">
-        <v>19</v>
+      <c r="L18" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M18" s="2">
-        <v>5.6</v>
-      </c>
-      <c r="N18" s="24">
-        <v>3.2</v>
+        <v>5.7</v>
+      </c>
+      <c r="N18" s="25">
+        <v>3.27</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -2611,34 +2653,34 @@
         <v>2.66</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F19" s="3">
-        <v>2.75</v>
+        <v>3.33</v>
       </c>
       <c r="G19">
-        <v>-0.25</v>
+        <v>-0.03</v>
       </c>
       <c r="H19">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="I19">
-        <v>-0.72</v>
+        <v>-0.1</v>
       </c>
       <c r="J19">
-        <v>0.25</v>
+        <v>0.46</v>
       </c>
       <c r="K19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="9" t="s">
-        <v>19</v>
+      <c r="L19" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M19" s="2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="N19" s="31">
-        <v>2.88</v>
+        <v>5</v>
+      </c>
+      <c r="N19" s="30">
+        <v>2.89</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -2675,13 +2717,13 @@
       <c r="K20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>21</v>
+      <c r="L20" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M20" s="2">
         <v>4.3</v>
       </c>
-      <c r="N20" s="32">
+      <c r="N20" s="31">
         <v>3.4</v>
       </c>
     </row>
@@ -2701,7 +2743,7 @@
       <c r="E21">
         <v>5</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>5.2</v>
       </c>
       <c r="G21">
@@ -2719,13 +2761,13 @@
       <c r="K21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M21" s="2">
-        <v>4.7</v>
-      </c>
-      <c r="N21" s="32">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N21" s="31">
         <v>3.4</v>
       </c>
     </row>
@@ -2763,13 +2805,13 @@
       <c r="K22" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L22" s="11" t="s">
-        <v>21</v>
+      <c r="L22" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M22" s="2">
         <v>4.3</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22" s="32">
         <v>3.2</v>
       </c>
     </row>
@@ -2789,7 +2831,7 @@
       <c r="E23">
         <v>6</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>3.33</v>
       </c>
       <c r="G23">
@@ -2807,13 +2849,13 @@
       <c r="K23" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L23" s="6" t="s">
-        <v>17</v>
+      <c r="L23" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M23" s="2">
         <v>5</v>
       </c>
-      <c r="N23" s="26">
+      <c r="N23" s="20">
         <v>3</v>
       </c>
     </row>
@@ -2831,22 +2873,22 @@
         <v>2.67</v>
       </c>
       <c r="E24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F24" s="3">
-        <v>2.7</v>
+        <v>2.64</v>
       </c>
       <c r="G24">
-        <v>-0.18</v>
+        <v>-0.21</v>
       </c>
       <c r="H24">
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="I24">
-        <v>-0.57999999999999996</v>
+        <v>-0.68</v>
       </c>
       <c r="J24">
-        <v>0.28999999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="K24" s="3" t="b">
         <v>0</v>
@@ -2857,7 +2899,7 @@
       <c r="M24" s="2">
         <v>5</v>
       </c>
-      <c r="N24" s="26">
+      <c r="N24" s="20">
         <v>3</v>
       </c>
     </row>
@@ -2875,33 +2917,33 @@
         <v>3.07</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F25" s="3">
-        <v>2.5</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="G25">
-        <v>-0.22</v>
+        <v>-0.31</v>
       </c>
       <c r="H25">
-        <v>1.08</v>
+        <v>1.02</v>
       </c>
       <c r="I25">
-        <v>-0.63</v>
+        <v>-0.94</v>
       </c>
       <c r="J25">
-        <v>0.27</v>
+        <v>0.19</v>
       </c>
       <c r="K25" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L25" s="9" t="s">
-        <v>19</v>
+      <c r="L25" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M25" s="2">
         <v>4.5</v>
       </c>
-      <c r="N25" s="26">
+      <c r="N25" s="20">
         <v>3</v>
       </c>
     </row>
@@ -2919,34 +2961,34 @@
         <v>2.42</v>
       </c>
       <c r="E26">
-        <v>10</v>
-      </c>
-      <c r="F26" s="8">
-        <v>3.7</v>
+        <v>11</v>
+      </c>
+      <c r="F26" s="7">
+        <v>3.55</v>
       </c>
       <c r="G26">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="H26">
-        <v>0.76</v>
+        <v>0.73</v>
       </c>
       <c r="I26">
-        <v>0.69</v>
+        <v>0.51</v>
       </c>
       <c r="J26">
-        <v>0.25</v>
+        <v>0.31</v>
       </c>
       <c r="K26" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L26" s="9" t="s">
-        <v>19</v>
+      <c r="L26" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M26" s="2">
         <v>5.3</v>
       </c>
-      <c r="N26" s="22">
-        <v>3.1</v>
+      <c r="N26" s="33">
+        <v>3.09</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
@@ -2963,34 +3005,34 @@
         <v>2.4</v>
       </c>
       <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27" s="8">
-        <v>3.6</v>
+        <v>11</v>
+      </c>
+      <c r="F27" s="7">
+        <v>3.36</v>
       </c>
       <c r="G27">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H27">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
       <c r="I27">
-        <v>0.63</v>
+        <v>0.34</v>
       </c>
       <c r="J27">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
       <c r="K27" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L27" s="9" t="s">
-        <v>19</v>
+      <c r="L27" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M27" s="2">
         <v>4.7</v>
       </c>
-      <c r="N27" s="22">
-        <v>3.1</v>
+      <c r="N27" s="23">
+        <v>3.18</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -3024,13 +3066,13 @@
       <c r="K28" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L28" s="21" t="s">
+      <c r="L28" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M28" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="N28" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N28" s="10">
         <v>4</v>
       </c>
     </row>
@@ -3048,34 +3090,34 @@
         <v>2.75</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F29" s="3">
-        <v>2.83</v>
+        <v>2.57</v>
       </c>
       <c r="G29">
-        <v>-0.08</v>
+        <v>-0.18</v>
       </c>
       <c r="H29">
-        <v>1.1200000000000001</v>
+        <v>1.04</v>
       </c>
       <c r="I29">
-        <v>-0.21</v>
+        <v>-0.47</v>
       </c>
       <c r="J29">
-        <v>0.42</v>
+        <v>0.33</v>
       </c>
       <c r="K29" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L29" s="6" t="s">
-        <v>17</v>
+      <c r="L29" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M29" s="2">
         <v>5</v>
       </c>
-      <c r="N29" s="28">
-        <v>2.67</v>
+      <c r="N29" s="34">
+        <v>2.71</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -3092,34 +3134,34 @@
         <v>2.68</v>
       </c>
       <c r="E30">
-        <v>10</v>
-      </c>
-      <c r="F30" s="8">
-        <v>3.4</v>
+        <v>11</v>
+      </c>
+      <c r="F30" s="7">
+        <v>3.18</v>
       </c>
       <c r="G30">
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
       <c r="H30">
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="I30">
-        <v>0.41</v>
+        <v>0.16</v>
       </c>
       <c r="J30">
-        <v>0.34</v>
+        <v>0.44</v>
       </c>
       <c r="K30" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L30" s="6" t="s">
-        <v>17</v>
+      <c r="L30" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M30" s="2">
         <v>4.5</v>
       </c>
-      <c r="N30" s="22">
-        <v>3.1</v>
+      <c r="N30" s="33">
+        <v>3.09</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -3156,13 +3198,13 @@
       <c r="K31" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L31" s="6" t="s">
-        <v>17</v>
+      <c r="L31" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M31" s="2">
         <v>5.5</v>
       </c>
-      <c r="N31" s="30">
+      <c r="N31" s="35">
         <v>3.22</v>
       </c>
     </row>
@@ -3175,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:G15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3184,47 +3226,47 @@
     <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="53" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52" t="s">
+    <row r="1" spans="1:14" s="60" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="59" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3242,34 +3284,34 @@
         <v>4.37</v>
       </c>
       <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" s="8">
-        <v>7.2</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="7">
+        <v>6.73</v>
       </c>
       <c r="G2">
-        <v>0.23</v>
+        <v>0.12</v>
       </c>
       <c r="H2">
-        <v>1.38</v>
+        <v>1.32</v>
       </c>
       <c r="I2">
-        <v>0.73</v>
+        <v>0.41</v>
       </c>
       <c r="J2">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
       <c r="K2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>19</v>
+      <c r="L2" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M2" s="2">
-        <v>12.8</v>
-      </c>
-      <c r="N2" s="33">
-        <v>3.1</v>
+        <v>12.9</v>
+      </c>
+      <c r="N2" s="36">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -3286,33 +3328,33 @@
         <v>3.78</v>
       </c>
       <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" s="8">
-        <v>6.7</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="7">
+        <v>6.27</v>
       </c>
       <c r="G3">
-        <v>0.37</v>
+        <v>0.26</v>
       </c>
       <c r="H3">
-        <v>1.2</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I3">
-        <v>1.19</v>
+        <v>0.87</v>
       </c>
       <c r="J3">
-        <v>0.13</v>
+        <v>0.2</v>
       </c>
       <c r="K3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>19</v>
+      <c r="L3" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M3" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="N3" s="25">
+        <v>9.6</v>
+      </c>
+      <c r="N3" s="36">
         <v>3</v>
       </c>
     </row>
@@ -3347,7 +3389,7 @@
       <c r="K4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M4" s="2">
@@ -3371,34 +3413,34 @@
         <v>3.26</v>
       </c>
       <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="F5" s="8">
-        <v>6.22</v>
+        <v>10</v>
+      </c>
+      <c r="F5" s="7">
+        <v>5.8</v>
       </c>
       <c r="G5">
-        <v>0.52</v>
+        <v>0.39</v>
       </c>
       <c r="H5">
-        <v>1.0900000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="I5">
-        <v>1.56</v>
+        <v>1.23</v>
       </c>
       <c r="J5">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="K5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>21</v>
+      <c r="L5" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M5" s="2">
         <v>8.6</v>
       </c>
-      <c r="N5" s="25">
-        <v>3</v>
+      <c r="N5" s="37">
+        <v>3.1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -3415,34 +3457,34 @@
         <v>3.08</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>3.38</v>
+        <v>3.22</v>
       </c>
       <c r="G6">
-        <v>-0.32</v>
+        <v>-0.37</v>
       </c>
       <c r="H6">
-        <v>1.0900000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="I6">
-        <v>-0.91</v>
+        <v>-1.1200000000000001</v>
       </c>
       <c r="J6">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="K6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>19</v>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M6" s="2">
         <v>7.7</v>
       </c>
-      <c r="N6" s="10">
-        <v>3.25</v>
+      <c r="N6" s="38">
+        <v>3.33</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -3459,33 +3501,33 @@
         <v>3.62</v>
       </c>
       <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7" s="8">
-        <v>5.6</v>
+        <v>11</v>
+      </c>
+      <c r="F7" s="7">
+        <v>5.18</v>
       </c>
       <c r="G7">
-        <v>0.34</v>
+        <v>0.23</v>
       </c>
       <c r="H7">
-        <v>1.1399999999999999</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I7">
-        <v>1.0900000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="J7">
-        <v>0.15</v>
+        <v>0.23</v>
       </c>
       <c r="K7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>19</v>
+      <c r="L7" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M7" s="2">
         <v>8.1</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="36">
         <v>3</v>
       </c>
     </row>
@@ -3503,34 +3545,34 @@
         <v>3.34</v>
       </c>
       <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8" s="8">
-        <v>5.3</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5.45</v>
       </c>
       <c r="G8">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="H8">
-        <v>1.06</v>
+        <v>1.01</v>
       </c>
       <c r="I8">
-        <v>0.95</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J8">
-        <v>0.18</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>19</v>
+      <c r="L8" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M8" s="2">
         <v>7.4</v>
       </c>
-      <c r="N8" s="34">
-        <v>3.2</v>
+      <c r="N8" s="16">
+        <v>3.18</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -3547,34 +3589,34 @@
         <v>3.61</v>
       </c>
       <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3">
-        <v>4.0999999999999996</v>
+        <v>11</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4.2699999999999996</v>
       </c>
       <c r="G9">
-        <v>-0.03</v>
+        <v>0.02</v>
       </c>
       <c r="H9">
-        <v>1.1399999999999999</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I9">
-        <v>-0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J9">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="K9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>17</v>
+      <c r="L9" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M9" s="2">
-        <v>7.6</v>
-      </c>
-      <c r="N9" s="33">
-        <v>3.1</v>
+        <v>7.5</v>
+      </c>
+      <c r="N9" s="39">
+        <v>3.09</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -3593,7 +3635,7 @@
       <c r="E10">
         <v>9</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>4.67</v>
       </c>
       <c r="G10">
@@ -3611,13 +3653,13 @@
       <c r="K10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>17</v>
+      <c r="L10" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M10" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="N10" s="35">
+        <v>8.4</v>
+      </c>
+      <c r="N10" s="38">
         <v>3.33</v>
       </c>
     </row>
@@ -3635,33 +3677,33 @@
         <v>3.66</v>
       </c>
       <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" s="8">
-        <v>4.3</v>
+        <v>11</v>
+      </c>
+      <c r="F11" s="7">
+        <v>4.3600000000000003</v>
       </c>
       <c r="G11">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="H11">
-        <v>1.1599999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I11">
-        <v>0.14000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J11">
-        <v>0.45</v>
+        <v>0.42</v>
       </c>
       <c r="K11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>17</v>
+      <c r="L11" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M11" s="2">
-        <v>7</v>
-      </c>
-      <c r="N11" s="25">
+        <v>6.9</v>
+      </c>
+      <c r="N11" s="36">
         <v>3</v>
       </c>
     </row>
@@ -3699,13 +3741,13 @@
       <c r="K12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="9" t="s">
-        <v>19</v>
+      <c r="L12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M12" s="2">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="N12" s="33">
+        <v>8.6</v>
+      </c>
+      <c r="N12" s="37">
         <v>3.1</v>
       </c>
     </row>
@@ -3723,34 +3765,34 @@
         <v>4.08</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F13" s="3">
-        <v>1.67</v>
+        <v>1.57</v>
       </c>
       <c r="G13">
-        <v>-0.59</v>
+        <v>-0.61</v>
       </c>
       <c r="H13">
-        <v>1.67</v>
+        <v>1.54</v>
       </c>
       <c r="I13">
-        <v>-1.43</v>
+        <v>-1.61</v>
       </c>
       <c r="J13">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="K13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="11" t="s">
-        <v>21</v>
+      <c r="L13" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M13" s="2">
         <v>6.8</v>
       </c>
-      <c r="N13" s="36">
-        <v>3.17</v>
+      <c r="N13" s="40">
+        <v>3.14</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -3787,13 +3829,13 @@
       <c r="K14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L14" s="9" t="s">
-        <v>19</v>
+      <c r="L14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M14" s="2">
         <v>6.2</v>
       </c>
-      <c r="N14" s="35">
+      <c r="N14" s="38">
         <v>3.33</v>
       </c>
     </row>
@@ -3811,34 +3853,34 @@
         <v>3.1</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" s="3">
-        <v>3.4</v>
+        <v>3.82</v>
       </c>
       <c r="G15">
-        <v>-0.18</v>
+        <v>-0.05</v>
       </c>
       <c r="H15">
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
       <c r="I15">
-        <v>-0.56999999999999995</v>
+        <v>-0.15</v>
       </c>
       <c r="J15">
-        <v>0.28999999999999998</v>
+        <v>0.44</v>
       </c>
       <c r="K15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>17</v>
+      <c r="L15" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M15" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="N15" s="33">
-        <v>3.1</v>
+      <c r="N15" s="39">
+        <v>3.09</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -3855,34 +3897,34 @@
         <v>2.59</v>
       </c>
       <c r="E16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>2.67</v>
+        <v>2.7</v>
       </c>
       <c r="G16">
-        <v>-0.47</v>
+        <v>-0.46</v>
       </c>
       <c r="H16">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="I16">
-        <v>-1.41</v>
+        <v>-1.45</v>
       </c>
       <c r="J16">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="K16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L16" s="9" t="s">
-        <v>19</v>
+      <c r="L16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M16" s="2">
         <v>5.3</v>
       </c>
-      <c r="N16" s="25">
-        <v>3</v>
+      <c r="N16" s="37">
+        <v>3.1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -3899,34 +3941,34 @@
         <v>3.34</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F17" s="3">
-        <v>3</v>
+        <v>2.71</v>
       </c>
       <c r="G17">
-        <v>-0.26</v>
+        <v>-0.35</v>
       </c>
       <c r="H17">
-        <v>1.36</v>
+        <v>1.26</v>
       </c>
       <c r="I17">
-        <v>-0.64</v>
+        <v>-0.92</v>
       </c>
       <c r="J17">
-        <v>0.28000000000000003</v>
+        <v>0.2</v>
       </c>
       <c r="K17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L17" s="9" t="s">
-        <v>19</v>
+      <c r="L17" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M17" s="2">
         <v>6.5</v>
       </c>
-      <c r="N17" s="36">
-        <v>3.17</v>
+      <c r="N17" s="41">
+        <v>3.29</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -3943,34 +3985,34 @@
         <v>2.73</v>
       </c>
       <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18" s="8">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="F18" s="7">
+        <v>4.09</v>
       </c>
       <c r="G18">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="H18">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="I18">
-        <v>0.18</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J18">
-        <v>0.43</v>
+        <v>0.39</v>
       </c>
       <c r="K18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="6" t="s">
-        <v>17</v>
+      <c r="L18" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M18" s="2">
         <v>6.5</v>
       </c>
-      <c r="N18" s="37">
-        <v>3.4</v>
+      <c r="N18" s="42">
+        <v>3.36</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -3987,33 +4029,33 @@
         <v>2.99</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" s="3">
-        <v>3.4</v>
+        <v>3.73</v>
       </c>
       <c r="G19">
-        <v>-0.13</v>
+        <v>-0.02</v>
       </c>
       <c r="H19">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="I19">
-        <v>-0.41</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="J19">
-        <v>0.34</v>
+        <v>0.47</v>
       </c>
       <c r="K19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="6" t="s">
-        <v>17</v>
+      <c r="L19" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M19" s="2">
         <v>7</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="36">
         <v>3</v>
       </c>
     </row>
@@ -4031,34 +4073,34 @@
         <v>4.12</v>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3">
-        <v>3.33</v>
+        <v>3.3</v>
       </c>
       <c r="G20">
         <v>-0.11</v>
       </c>
       <c r="H20">
-        <v>1.37</v>
+        <v>1.3</v>
       </c>
       <c r="I20">
-        <v>-0.32</v>
+        <v>-0.36</v>
       </c>
       <c r="J20">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="K20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="6" t="s">
-        <v>17</v>
+      <c r="L20" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M20" s="2">
         <v>7.7</v>
       </c>
-      <c r="N20" s="38">
-        <v>3.11</v>
+      <c r="N20" s="36">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -4075,34 +4117,34 @@
         <v>3.04</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3">
-        <v>3.44</v>
+        <v>3.7</v>
       </c>
       <c r="G21">
-        <v>-0.11</v>
+        <v>-0.02</v>
       </c>
       <c r="H21">
-        <v>1.01</v>
+        <v>0.96</v>
       </c>
       <c r="I21">
-        <v>-0.32</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="J21">
-        <v>0.38</v>
+        <v>0.47</v>
       </c>
       <c r="K21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>17</v>
+      <c r="L21" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M21" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="N21" s="38">
-        <v>3.11</v>
+        <v>7.4</v>
+      </c>
+      <c r="N21" s="36">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -4139,13 +4181,13 @@
       <c r="K22" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L22" s="11" t="s">
-        <v>21</v>
+      <c r="L22" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M22" s="2">
         <v>7.3</v>
       </c>
-      <c r="N22" s="36">
+      <c r="N22" s="43">
         <v>3.17</v>
       </c>
     </row>
@@ -4163,19 +4205,19 @@
         <v>2.87</v>
       </c>
       <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="F23" s="8">
-        <v>5.8</v>
+        <v>11</v>
+      </c>
+      <c r="F23" s="7">
+        <v>5.73</v>
       </c>
       <c r="G23">
-        <v>0.77</v>
+        <v>0.74</v>
       </c>
       <c r="H23">
-        <v>0.91</v>
+        <v>0.86</v>
       </c>
       <c r="I23">
-        <v>2.42</v>
+        <v>2.46</v>
       </c>
       <c r="J23">
         <v>0.02</v>
@@ -4183,14 +4225,14 @@
       <c r="K23" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L23" s="11" t="s">
-        <v>21</v>
+      <c r="L23" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M23" s="2">
         <v>6.7</v>
       </c>
-      <c r="N23" s="33">
-        <v>3.1</v>
+      <c r="N23" s="39">
+        <v>3.09</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
@@ -4207,34 +4249,34 @@
         <v>3.23</v>
       </c>
       <c r="E24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24" s="3">
-        <v>2.29</v>
+        <v>2.25</v>
       </c>
       <c r="G24">
-        <v>-0.4</v>
+        <v>-0.41</v>
       </c>
       <c r="H24">
-        <v>1.22</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I24">
-        <v>-1.05</v>
+        <v>-1.1499999999999999</v>
       </c>
       <c r="J24">
-        <v>0.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K24" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L24" s="9" t="s">
-        <v>19</v>
+      <c r="L24" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M24" s="2">
         <v>5.4</v>
       </c>
-      <c r="N24" s="25">
-        <v>3</v>
+      <c r="N24" s="44">
+        <v>3.25</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -4251,34 +4293,34 @@
         <v>2.61</v>
       </c>
       <c r="E25">
-        <v>9</v>
-      </c>
-      <c r="F25" s="8">
-        <v>4.1100000000000003</v>
+        <v>10</v>
+      </c>
+      <c r="F25" s="7">
+        <v>3.9</v>
       </c>
       <c r="G25">
-        <v>0.22</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H25">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="I25">
-        <v>0.66</v>
+        <v>0.44</v>
       </c>
       <c r="J25">
-        <v>0.27</v>
+        <v>0.34</v>
       </c>
       <c r="K25" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L25" s="9" t="s">
-        <v>19</v>
+      <c r="L25" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M25" s="2">
-        <v>6.3</v>
-      </c>
-      <c r="N25" s="39">
-        <v>3.22</v>
+        <v>6.2</v>
+      </c>
+      <c r="N25" s="45">
+        <v>3.2</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -4295,19 +4337,19 @@
         <v>2.11</v>
       </c>
       <c r="E26">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3">
-        <v>2.33</v>
+        <v>2.4</v>
       </c>
       <c r="G26">
-        <v>-0.55000000000000004</v>
+        <v>-0.51</v>
       </c>
       <c r="H26">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="I26">
-        <v>-1.64</v>
+        <v>-1.63</v>
       </c>
       <c r="J26">
         <v>7.0000000000000007E-2</v>
@@ -4315,14 +4357,14 @@
       <c r="K26" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L26" s="11" t="s">
-        <v>21</v>
+      <c r="L26" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M26" s="2">
         <v>5.9</v>
       </c>
-      <c r="N26" s="39">
-        <v>3.22</v>
+      <c r="N26" s="45">
+        <v>3.2</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
@@ -4339,19 +4381,19 @@
         <v>2.75</v>
       </c>
       <c r="E27">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F27" s="3">
-        <v>2.4</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="G27">
-        <v>-0.39</v>
+        <v>-0.37</v>
       </c>
       <c r="H27">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="I27">
-        <v>-1.22</v>
+        <v>-1.21</v>
       </c>
       <c r="J27">
         <v>0.13</v>
@@ -4359,14 +4401,14 @@
       <c r="K27" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L27" s="9" t="s">
-        <v>19</v>
+      <c r="L27" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M27" s="2">
-        <v>5.8</v>
-      </c>
-      <c r="N27" s="34">
-        <v>3.2</v>
+        <v>5.7</v>
+      </c>
+      <c r="N27" s="16">
+        <v>3.18</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -4383,34 +4425,34 @@
         <v>2.09</v>
       </c>
       <c r="E28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F28" s="3">
-        <v>2.9</v>
+        <v>2.91</v>
       </c>
       <c r="G28">
         <v>-0.26</v>
       </c>
       <c r="H28">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="I28">
-        <v>-0.84</v>
+        <v>-0.86</v>
       </c>
       <c r="J28">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="K28" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L28" s="9" t="s">
-        <v>19</v>
+      <c r="L28" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M28" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="N28" s="33">
-        <v>3.1</v>
+        <v>5.4</v>
+      </c>
+      <c r="N28" s="16">
+        <v>3.18</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
@@ -4427,34 +4469,34 @@
         <v>2.83</v>
       </c>
       <c r="E29">
-        <v>8</v>
-      </c>
-      <c r="F29" s="8">
-        <v>3.62</v>
+        <v>9</v>
+      </c>
+      <c r="F29" s="7">
+        <v>3.44</v>
       </c>
       <c r="G29">
-        <v>7.0000000000000007E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="I29">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="J29">
-        <v>0.42</v>
+        <v>0.49</v>
       </c>
       <c r="K29" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L29" s="6" t="s">
-        <v>17</v>
+      <c r="L29" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="M29" s="2">
         <v>6.3</v>
       </c>
-      <c r="N29" s="14">
-        <v>3.5</v>
+      <c r="N29" s="10">
+        <v>3.44</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -4471,34 +4513,34 @@
         <v>2.91</v>
       </c>
       <c r="E30">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F30" s="3">
-        <v>1.75</v>
+        <v>1.78</v>
       </c>
       <c r="G30">
-        <v>-0.55000000000000004</v>
+        <v>-0.54</v>
       </c>
       <c r="H30">
-        <v>1.03</v>
+        <v>0.97</v>
       </c>
       <c r="I30">
-        <v>-1.55</v>
+        <v>-1.62</v>
       </c>
       <c r="J30">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K30" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L30" s="11" t="s">
-        <v>21</v>
+      <c r="L30" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M30" s="2">
         <v>5.7</v>
       </c>
-      <c r="N30" s="40">
-        <v>3.12</v>
+      <c r="N30" s="46">
+        <v>3.11</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -4515,34 +4557,34 @@
         <v>2.77</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F31" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="G31">
-        <v>-0.37</v>
+        <v>-0.41</v>
       </c>
       <c r="H31">
-        <v>0.88</v>
+        <v>0.84</v>
       </c>
       <c r="I31">
-        <v>-1.1599999999999999</v>
+        <v>-1.35</v>
       </c>
       <c r="J31">
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="K31" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L31" s="9" t="s">
-        <v>19</v>
+      <c r="L31" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M31" s="2">
         <v>7.1</v>
       </c>
-      <c r="N31" s="34">
-        <v>3.2</v>
+      <c r="N31" s="47">
+        <v>3.27</v>
       </c>
     </row>
   </sheetData>
@@ -4554,8 +4596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="N24" sqref="A23:N24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4563,47 +4605,47 @@
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="53" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52" t="s">
+    <row r="1" spans="1:14" s="60" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="59" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4621,34 +4663,34 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" s="8">
-        <v>6.8</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6.27</v>
       </c>
       <c r="G2">
-        <v>0.04</v>
+        <v>-0.08</v>
       </c>
       <c r="H2">
-        <v>1.38</v>
+        <v>1.31</v>
       </c>
       <c r="I2">
-        <v>0.12</v>
+        <v>-0.27</v>
       </c>
       <c r="J2">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="K2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>17</v>
+      <c r="L2" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M2" s="2">
         <v>14</v>
       </c>
-      <c r="N2" s="41">
-        <v>3.1</v>
+      <c r="N2" s="48">
+        <v>3.09</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -4665,34 +4707,34 @@
         <v>3.38</v>
       </c>
       <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="F3" s="8">
-        <v>4.4400000000000004</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="7">
+        <v>4.2</v>
       </c>
       <c r="G3">
-        <v>0.12</v>
+        <v>0.05</v>
       </c>
       <c r="H3">
-        <v>1.1299999999999999</v>
+        <v>1.07</v>
       </c>
       <c r="I3">
-        <v>0.36</v>
+        <v>0.15</v>
       </c>
       <c r="J3">
-        <v>0.36</v>
+        <v>0.44</v>
       </c>
       <c r="K3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>17</v>
+      <c r="L3" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M3" s="2">
         <v>7.8</v>
       </c>
-      <c r="N3" s="40">
-        <v>3.22</v>
+      <c r="N3" s="49">
+        <v>3.3</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -4729,13 +4771,13 @@
       <c r="K4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>19</v>
+      <c r="L4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M4" s="2">
-        <v>7.9</v>
-      </c>
-      <c r="N4" s="14">
+        <v>7.8</v>
+      </c>
+      <c r="N4" s="10">
         <v>3.43</v>
       </c>
     </row>
@@ -4770,13 +4812,13 @@
       <c r="K5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>21</v>
+      <c r="L5" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M5" s="2">
         <v>7.4</v>
       </c>
-      <c r="N5" s="42">
+      <c r="N5" s="50">
         <v>3</v>
       </c>
     </row>
@@ -4796,7 +4838,7 @@
       <c r="E6">
         <v>8</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>4.75</v>
       </c>
       <c r="G6">
@@ -4814,13 +4856,13 @@
       <c r="K6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>19</v>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M6" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="N6" s="43">
+        <v>7.4</v>
+      </c>
+      <c r="N6" s="23">
         <v>3.12</v>
       </c>
     </row>
@@ -4838,33 +4880,33 @@
         <v>2.48</v>
       </c>
       <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7" s="8">
-        <v>6.4</v>
+        <v>11</v>
+      </c>
+      <c r="F7" s="7">
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>1.1000000000000001</v>
+        <v>0.94</v>
       </c>
       <c r="H7">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="I7">
-        <v>3.49</v>
+        <v>3.12</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="2">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="N7" s="42">
+        <v>8.4</v>
+      </c>
+      <c r="N7" s="50">
         <v>3</v>
       </c>
     </row>
@@ -4882,34 +4924,34 @@
         <v>2.77</v>
       </c>
       <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8" s="8">
-        <v>3.8</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="7">
+        <v>3.64</v>
       </c>
       <c r="G8">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="H8">
-        <v>0.88</v>
+        <v>0.84</v>
       </c>
       <c r="I8">
-        <v>0.32</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J8">
-        <v>0.38</v>
+        <v>0.44</v>
       </c>
       <c r="K8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>17</v>
+      <c r="L8" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M8" s="2">
         <v>6.4</v>
       </c>
-      <c r="N8" s="41">
-        <v>3.1</v>
+      <c r="N8" s="40">
+        <v>3.27</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -4926,34 +4968,34 @@
         <v>2.8</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="3">
-        <v>2.25</v>
+        <v>2.11</v>
       </c>
       <c r="G9">
-        <v>-0.44</v>
+        <v>-0.49</v>
       </c>
       <c r="H9">
-        <v>0.99</v>
+        <v>0.93</v>
       </c>
       <c r="I9">
-        <v>-1.24</v>
+        <v>-1.46</v>
       </c>
       <c r="J9">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="K9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>19</v>
+      <c r="L9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M9" s="2">
         <v>7.2</v>
       </c>
-      <c r="N9" s="43">
-        <v>3.12</v>
+      <c r="N9" s="50">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -4970,34 +5012,34 @@
         <v>2.85</v>
       </c>
       <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10" s="8">
-        <v>4.78</v>
+        <v>10</v>
+      </c>
+      <c r="F10" s="7">
+        <v>4.5</v>
       </c>
       <c r="G10">
-        <v>0.56000000000000005</v>
+        <v>0.47</v>
       </c>
       <c r="H10">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="I10">
-        <v>1.69</v>
+        <v>1.47</v>
       </c>
       <c r="J10">
-        <v>7.0000000000000007E-2</v>
+        <v>0.09</v>
       </c>
       <c r="K10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="11" t="s">
-        <v>21</v>
+      <c r="L10" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M10" s="2">
-        <v>7.4</v>
-      </c>
-      <c r="N10" s="44">
-        <v>3.11</v>
+        <v>7.5</v>
+      </c>
+      <c r="N10" s="50">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -5014,34 +5056,34 @@
         <v>2.82</v>
       </c>
       <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11" s="8">
-        <v>3.88</v>
+        <v>9</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3.67</v>
       </c>
       <c r="G11">
-        <v>0.27</v>
+        <v>0.2</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="I11">
-        <v>0.77</v>
+        <v>0.59</v>
       </c>
       <c r="J11">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="9" t="s">
-        <v>19</v>
+      <c r="L11" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M11" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="N11" s="45">
-        <v>3.38</v>
+        <v>6.4</v>
+      </c>
+      <c r="N11" s="44">
+        <v>3.33</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -5058,34 +5100,34 @@
         <v>2.42</v>
       </c>
       <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3">
-        <v>2.8</v>
+        <v>11</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>-0.08</v>
+        <v>0.01</v>
       </c>
       <c r="H12">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="I12">
-        <v>-0.24</v>
+        <v>0.02</v>
       </c>
       <c r="J12">
-        <v>0.41</v>
+        <v>0.49</v>
       </c>
       <c r="K12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="6" t="s">
-        <v>17</v>
+      <c r="L12" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="M12" s="2">
         <v>5.8</v>
       </c>
-      <c r="N12" s="46">
-        <v>3.2</v>
+      <c r="N12" s="51">
+        <v>3.18</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -5102,34 +5144,34 @@
         <v>2.67</v>
       </c>
       <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13" s="8">
-        <v>3.4</v>
+        <v>11</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3.27</v>
       </c>
       <c r="G13">
-        <v>0.19</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H13">
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="I13">
-        <v>0.59</v>
+        <v>0.46</v>
       </c>
       <c r="J13">
-        <v>0.28000000000000003</v>
+        <v>0.33</v>
       </c>
       <c r="K13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>17</v>
+      <c r="L13" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M13" s="2">
         <v>6</v>
       </c>
-      <c r="N13" s="47">
-        <v>3.4</v>
+      <c r="N13" s="52">
+        <v>3.36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -5166,13 +5208,13 @@
       <c r="K14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L14" s="9" t="s">
-        <v>19</v>
+      <c r="L14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M14" s="2">
         <v>5.8</v>
       </c>
-      <c r="N14" s="45">
+      <c r="N14" s="53">
         <v>3.38</v>
       </c>
     </row>
@@ -5190,34 +5232,34 @@
         <v>2.95</v>
       </c>
       <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15" s="8">
-        <v>4.8</v>
+        <v>11</v>
+      </c>
+      <c r="F15" s="7">
+        <v>4.55</v>
       </c>
       <c r="G15">
-        <v>0.65</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H15">
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="I15">
-        <v>2.0699999999999998</v>
+        <v>1.88</v>
       </c>
       <c r="J15">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="K15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="11" t="s">
-        <v>21</v>
+      <c r="L15" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M15" s="2">
-        <v>7.1</v>
-      </c>
-      <c r="N15" s="41">
-        <v>3.1</v>
+        <v>7.2</v>
+      </c>
+      <c r="N15" s="48">
+        <v>3.09</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -5234,34 +5276,34 @@
         <v>2.58</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="G16">
-        <v>-0.67</v>
+        <v>-0.72</v>
       </c>
       <c r="H16">
-        <v>0.98</v>
+        <v>0.91</v>
       </c>
       <c r="I16">
-        <v>-1.78</v>
+        <v>-2.04</v>
       </c>
       <c r="J16">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="K16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L16" s="11" t="s">
-        <v>21</v>
+      <c r="L16" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M16" s="2">
-        <v>5.7</v>
-      </c>
-      <c r="N16" s="48">
-        <v>3.29</v>
+        <v>5.6</v>
+      </c>
+      <c r="N16" s="37">
+        <v>3.25</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -5298,13 +5340,13 @@
       <c r="K17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M17" s="2">
         <v>5</v>
       </c>
-      <c r="N17" s="49">
+      <c r="N17" s="37">
         <v>3.25</v>
       </c>
     </row>
@@ -5322,34 +5364,34 @@
         <v>1.95</v>
       </c>
       <c r="E18">
-        <v>7</v>
-      </c>
-      <c r="F18" s="8">
-        <v>3.29</v>
+        <v>8</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3.12</v>
       </c>
       <c r="G18">
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="H18">
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="I18">
-        <v>0.79</v>
+        <v>0.61</v>
       </c>
       <c r="J18">
-        <v>0.23</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="9" t="s">
-        <v>19</v>
+      <c r="L18" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M18" s="2">
         <v>5.8</v>
       </c>
-      <c r="N18" s="50">
-        <v>3.14</v>
+      <c r="N18" s="23">
+        <v>3.12</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -5366,34 +5408,34 @@
         <v>2.23</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F19" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="G19">
-        <v>-0.64</v>
+        <v>-0.65</v>
       </c>
       <c r="H19">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="I19">
-        <v>-1.81</v>
+        <v>-1.94</v>
       </c>
       <c r="J19">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="K19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="11" t="s">
-        <v>21</v>
+      <c r="L19" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M19" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="N19" s="49">
-        <v>3.25</v>
+        <v>6.4</v>
+      </c>
+      <c r="N19" s="54">
+        <v>3.22</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -5410,34 +5452,34 @@
         <v>2.27</v>
       </c>
       <c r="E20">
-        <v>9</v>
-      </c>
-      <c r="F20" s="8">
-        <v>3.67</v>
+        <v>10</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3.4</v>
       </c>
       <c r="G20">
-        <v>0.53</v>
+        <v>0.41</v>
       </c>
       <c r="H20">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
       <c r="I20">
-        <v>1.59</v>
+        <v>1.31</v>
       </c>
       <c r="J20">
-        <v>7.0000000000000007E-2</v>
+        <v>0.11</v>
       </c>
       <c r="K20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>21</v>
+      <c r="L20" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M20" s="2">
         <v>5.5</v>
       </c>
-      <c r="N20" s="44">
-        <v>3.11</v>
+      <c r="N20" s="50">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -5454,34 +5496,34 @@
         <v>2.23</v>
       </c>
       <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21" s="8">
-        <v>3.7</v>
+        <v>11</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3.55</v>
       </c>
       <c r="G21">
-        <v>0.56000000000000005</v>
+        <v>0.49</v>
       </c>
       <c r="H21">
-        <v>0.7</v>
+        <v>0.67</v>
       </c>
       <c r="I21">
-        <v>1.77</v>
+        <v>1.62</v>
       </c>
       <c r="J21">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L21" s="11" t="s">
-        <v>21</v>
+      <c r="L21" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M21" s="2">
         <v>5.9</v>
       </c>
-      <c r="N21" s="41">
-        <v>3.1</v>
+      <c r="N21" s="48">
+        <v>3.09</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -5498,34 +5540,34 @@
         <v>2.08</v>
       </c>
       <c r="E22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3">
-        <v>1.44</v>
+        <v>1.3</v>
       </c>
       <c r="G22">
-        <v>-0.47</v>
+        <v>-0.54</v>
       </c>
       <c r="H22">
-        <v>0.69</v>
+        <v>0.66</v>
       </c>
       <c r="I22">
-        <v>-1.42</v>
+        <v>-1.71</v>
       </c>
       <c r="J22">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="K22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M22" s="2">
-        <v>5.3</v>
-      </c>
-      <c r="N22" s="40">
-        <v>3.22</v>
+        <v>5.2</v>
+      </c>
+      <c r="N22" s="49">
+        <v>3.3</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
@@ -5544,7 +5586,7 @@
       <c r="E23">
         <v>3</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>2.67</v>
       </c>
       <c r="G23">
@@ -5562,13 +5604,13 @@
       <c r="K23" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L23" s="6" t="s">
-        <v>17</v>
+      <c r="L23" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M23" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N23" s="51">
+      <c r="N23" s="19">
         <v>2.67</v>
       </c>
     </row>
@@ -5586,34 +5628,34 @@
         <v>2.13</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F24" s="3">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="G24">
-        <v>-0.1</v>
+        <v>-0.18</v>
       </c>
       <c r="H24">
-        <v>0.95</v>
+        <v>0.87</v>
       </c>
       <c r="I24">
-        <v>-0.22</v>
+        <v>-0.44</v>
       </c>
       <c r="J24">
-        <v>0.42</v>
+        <v>0.34</v>
       </c>
       <c r="K24" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L24" s="6" t="s">
-        <v>17</v>
+      <c r="L24" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M24" s="2">
         <v>4.8</v>
       </c>
-      <c r="N24" s="19">
-        <v>2.6</v>
+      <c r="N24" s="55">
+        <v>2.83</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -5632,7 +5674,7 @@
       <c r="E25">
         <v>9</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>2.56</v>
       </c>
       <c r="G25">
@@ -5650,13 +5692,13 @@
       <c r="K25" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L25" s="9" t="s">
-        <v>19</v>
+      <c r="L25" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M25" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N25" s="44">
+      <c r="N25" s="56">
         <v>3.11</v>
       </c>
     </row>
@@ -5674,34 +5716,34 @@
         <v>1.84</v>
       </c>
       <c r="E26">
-        <v>7</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1.86</v>
+        <v>8</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2.38</v>
       </c>
       <c r="G26">
-        <v>-0.14000000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H26">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="I26">
-        <v>-0.38</v>
+        <v>0.39</v>
       </c>
       <c r="J26">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="K26" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L26" s="6" t="s">
-        <v>17</v>
+      <c r="L26" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M26" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N26" s="50">
-        <v>3.14</v>
+      <c r="N26" s="23">
+        <v>3.12</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
@@ -5718,34 +5760,34 @@
         <v>1.49</v>
       </c>
       <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27" s="8">
-        <v>2.4</v>
+        <v>11</v>
+      </c>
+      <c r="F27" s="7">
+        <v>2.27</v>
       </c>
       <c r="G27">
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
       <c r="H27">
-        <v>0.47</v>
+        <v>0.45</v>
       </c>
       <c r="I27">
-        <v>0.85</v>
+        <v>0.61</v>
       </c>
       <c r="J27">
-        <v>0.21</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K27" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L27" s="9" t="s">
-        <v>19</v>
+      <c r="L27" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M27" s="2">
         <v>5.3</v>
       </c>
-      <c r="N27" s="47">
-        <v>3.4</v>
+      <c r="N27" s="52">
+        <v>3.36</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -5782,13 +5824,13 @@
       <c r="K28" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L28" s="9" t="s">
-        <v>19</v>
+      <c r="L28" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M28" s="2">
         <v>4.7</v>
       </c>
-      <c r="N28" s="46">
+      <c r="N28" s="57">
         <v>3.2</v>
       </c>
     </row>
@@ -5806,19 +5848,19 @@
         <v>1.25</v>
       </c>
       <c r="E29">
-        <v>10</v>
-      </c>
-      <c r="F29" s="8">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="F29" s="7">
+        <v>2.91</v>
       </c>
       <c r="G29">
-        <v>0.85</v>
+        <v>0.78</v>
       </c>
       <c r="H29">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="I29">
-        <v>2.68</v>
+        <v>2.57</v>
       </c>
       <c r="J29">
         <v>0.01</v>
@@ -5826,14 +5868,14 @@
       <c r="K29" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L29" s="21" t="s">
-        <v>38</v>
+      <c r="L29" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M29" s="2">
         <v>5.5</v>
       </c>
-      <c r="N29" s="47">
-        <v>3.4</v>
+      <c r="N29" s="40">
+        <v>3.27</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -5850,19 +5892,19 @@
         <v>2.1</v>
       </c>
       <c r="E30">
-        <v>10</v>
-      </c>
-      <c r="F30" s="8">
-        <v>4.2</v>
+        <v>11</v>
+      </c>
+      <c r="F30" s="7">
+        <v>4</v>
       </c>
       <c r="G30">
-        <v>1.08</v>
+        <v>0.98</v>
       </c>
       <c r="H30">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="I30">
-        <v>3.41</v>
+        <v>3.26</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -5870,14 +5912,14 @@
       <c r="K30" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L30" s="21" t="s">
+      <c r="L30" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M30" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="N30" s="46">
-        <v>3.2</v>
+        <v>5.6</v>
+      </c>
+      <c r="N30" s="40">
+        <v>3.27</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -5894,34 +5936,34 @@
         <v>1.6</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F31" s="3">
-        <v>1</v>
+        <v>1.17</v>
       </c>
       <c r="G31">
-        <v>-0.57999999999999996</v>
+        <v>-0.48</v>
       </c>
       <c r="H31">
-        <v>0.72</v>
+        <v>0.65</v>
       </c>
       <c r="I31">
-        <v>-1.3</v>
+        <v>-1.17</v>
       </c>
       <c r="J31">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="K31" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L31" s="11" t="s">
-        <v>21</v>
+      <c r="L31" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="M31" s="2">
         <v>5.3</v>
       </c>
-      <c r="N31" s="46">
-        <v>3.2</v>
+      <c r="N31" s="58">
+        <v>3.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>